<commit_message>
definição das classes a serem testadas.
</commit_message>
<xml_diff>
--- a/metricas de complexidade.xlsx
+++ b/metricas de complexidade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoSpring-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoSpring\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +105,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,10 +142,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +430,7 @@
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,54 +465,54 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>18</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>23</v>
       </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>15</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>21</v>
       </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>0</v>
       </c>
     </row>
@@ -588,28 +595,28 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>17</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>6</v>
       </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calculo das métricas de McCabe
</commit_message>
<xml_diff>
--- a/metricas de complexidade.xlsx
+++ b/metricas de complexidade.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metricas CK &amp; LK" sheetId="1" r:id="rId1"/>
+    <sheet name="CC McCabe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
   <si>
     <t>WMC</t>
   </si>
@@ -72,6 +73,237 @@
   </si>
   <si>
     <t>EstadoProduto</t>
+  </si>
+  <si>
+    <t>AutorizadorInterceptor</t>
+  </si>
+  <si>
+    <t>ClienteDao</t>
+  </si>
+  <si>
+    <t>FornecedorDao</t>
+  </si>
+  <si>
+    <t>ItemDao</t>
+  </si>
+  <si>
+    <t>PedidoDao</t>
+  </si>
+  <si>
+    <t>ProdutoDao</t>
+  </si>
+  <si>
+    <t>IndexController</t>
+  </si>
+  <si>
+    <t>ClienteController</t>
+  </si>
+  <si>
+    <t>FornecedorController</t>
+  </si>
+  <si>
+    <t>ProdutoController</t>
+  </si>
+  <si>
+    <t>CarrinhoController</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Método</t>
+  </si>
+  <si>
+    <t>C.C.</t>
+  </si>
+  <si>
+    <t>preHandle</t>
+  </si>
+  <si>
+    <t>adicionarProdutoCarrinho</t>
+  </si>
+  <si>
+    <t>listaProdutosCarrinho</t>
+  </si>
+  <si>
+    <t>executarCompra</t>
+  </si>
+  <si>
+    <t>cadastrarCliente</t>
+  </si>
+  <si>
+    <t>loginCliente</t>
+  </si>
+  <si>
+    <t>efetuaLogin</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>salvarCliente</t>
+  </si>
+  <si>
+    <t>FonecedorController</t>
+  </si>
+  <si>
+    <t>cadastrarFornecedor</t>
+  </si>
+  <si>
+    <t>salvarFornecedor</t>
+  </si>
+  <si>
+    <t>inicio</t>
+  </si>
+  <si>
+    <t>detalharProduto</t>
+  </si>
+  <si>
+    <t>cadastrarProduto</t>
+  </si>
+  <si>
+    <t>cadastrarProdutoPost</t>
+  </si>
+  <si>
+    <t>atualizarProduto</t>
+  </si>
+  <si>
+    <t>atualizarProdutoPost</t>
+  </si>
+  <si>
+    <t>listarProdutos</t>
+  </si>
+  <si>
+    <t>deletarProduto</t>
+  </si>
+  <si>
+    <t>buscarProdutoPelaMarca</t>
+  </si>
+  <si>
+    <t>ClienteDAO</t>
+  </si>
+  <si>
+    <t>persistCliente</t>
+  </si>
+  <si>
+    <t>getInstance</t>
+  </si>
+  <si>
+    <t>getById</t>
+  </si>
+  <si>
+    <t>listaCliente</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>removeById</t>
+  </si>
+  <si>
+    <t>logarCliente</t>
+  </si>
+  <si>
+    <t>FornecedorDAO</t>
+  </si>
+  <si>
+    <t>persistFornecedor</t>
+  </si>
+  <si>
+    <t>listFornecedor</t>
+  </si>
+  <si>
+    <t>ItemDAO</t>
+  </si>
+  <si>
+    <t>getInstace</t>
+  </si>
+  <si>
+    <t>persistProduto</t>
+  </si>
+  <si>
+    <t>listItem</t>
+  </si>
+  <si>
+    <t>PedidoDAO</t>
+  </si>
+  <si>
+    <t>persistPedido</t>
+  </si>
+  <si>
+    <t>listPedido</t>
+  </si>
+  <si>
+    <t>ProdutoDAO</t>
+  </si>
+  <si>
+    <t>getByMarca</t>
+  </si>
+  <si>
+    <t>listProduto</t>
+  </si>
+  <si>
+    <t>ItemForm</t>
+  </si>
+  <si>
+    <t>getItens</t>
+  </si>
+  <si>
+    <t>setItens</t>
+  </si>
+  <si>
+    <t>getId</t>
+  </si>
+  <si>
+    <t>getNome</t>
+  </si>
+  <si>
+    <t>setNome</t>
+  </si>
+  <si>
+    <t>getCpf</t>
+  </si>
+  <si>
+    <t>setCpf</t>
+  </si>
+  <si>
+    <t>getEmail</t>
+  </si>
+  <si>
+    <t>setEmail</t>
+  </si>
+  <si>
+    <t>getSenha</t>
+  </si>
+  <si>
+    <t>setSenha</t>
+  </si>
+  <si>
+    <t>getEndereco</t>
+  </si>
+  <si>
+    <t>setEndereco</t>
+  </si>
+  <si>
+    <t>getTipoCliente</t>
+  </si>
+  <si>
+    <t>setTipoCliente</t>
+  </si>
+  <si>
+    <t>setId</t>
+  </si>
+  <si>
+    <t>getPedidos</t>
+  </si>
+  <si>
+    <t>setPedidos</t>
+  </si>
+  <si>
+    <t>getTipoClienteString</t>
   </si>
 </sst>
 </file>
@@ -95,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +343,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,11 +392,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +682,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H10"/>
+  <dimension ref="A2:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -672,6 +927,1159 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complexidade Ciclomática de McCabe, finalização.
</commit_message>
<xml_diff>
--- a/metricas de complexidade.xlsx
+++ b/metricas de complexidade.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="132">
   <si>
     <t>WMC</t>
   </si>
@@ -304,6 +304,123 @@
   </si>
   <si>
     <t>getTipoClienteString</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>getRua</t>
+  </si>
+  <si>
+    <t>setRua</t>
+  </si>
+  <si>
+    <t>getCidade</t>
+  </si>
+  <si>
+    <t>setCidade</t>
+  </si>
+  <si>
+    <t>getEstado</t>
+  </si>
+  <si>
+    <t>setEstado</t>
+  </si>
+  <si>
+    <t>getCep</t>
+  </si>
+  <si>
+    <t>setCep</t>
+  </si>
+  <si>
+    <t>getPais</t>
+  </si>
+  <si>
+    <t>setPais</t>
+  </si>
+  <si>
+    <t>getFornecedor</t>
+  </si>
+  <si>
+    <t>setFornecedor</t>
+  </si>
+  <si>
+    <t>getProdutos</t>
+  </si>
+  <si>
+    <t>setProdutos</t>
+  </si>
+  <si>
+    <t>getQuantidade</t>
+  </si>
+  <si>
+    <t>setQuantidade</t>
+  </si>
+  <si>
+    <t>getPedido</t>
+  </si>
+  <si>
+    <t>setPedido</t>
+  </si>
+  <si>
+    <t>getProduto</t>
+  </si>
+  <si>
+    <t>setProduto</t>
+  </si>
+  <si>
+    <t>getData</t>
+  </si>
+  <si>
+    <t>setData</t>
+  </si>
+  <si>
+    <t>getCliente</t>
+  </si>
+  <si>
+    <t>setCliente</t>
+  </si>
+  <si>
+    <t>getMarca</t>
+  </si>
+  <si>
+    <t>setMarca</t>
+  </si>
+  <si>
+    <t>getModelo</t>
+  </si>
+  <si>
+    <t>setModelo</t>
+  </si>
+  <si>
+    <t>getNumero</t>
+  </si>
+  <si>
+    <t>setNumero</t>
+  </si>
+  <si>
+    <t>getPreco</t>
+  </si>
+  <si>
+    <t>setPreco</t>
+  </si>
+  <si>
+    <t>getCaminhoImagem</t>
+  </si>
+  <si>
+    <t>setCaminhoImagem</t>
+  </si>
+  <si>
+    <t>getEstadoProduto</t>
+  </si>
+  <si>
+    <t>setEstadoProduto</t>
+  </si>
+  <si>
+    <t>JPAUtil</t>
+  </si>
+  <si>
+    <t>getEntityManager</t>
   </si>
 </sst>
 </file>
@@ -327,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +481,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -392,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -402,6 +531,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1221,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C78"/>
+  <dimension ref="A2:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1460,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2077,6 +2208,611 @@
         <v>92</v>
       </c>
       <c r="C78" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C90" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C91" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C92" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C93" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C95" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C96" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C97" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C98" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C99" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C100" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C101" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C102" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C104" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C105" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C106" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C109" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C110" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C112" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C113" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C114" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C115" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C116" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C117" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C118" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C119" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C121" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C123" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C124" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C125" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C126" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C127" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C128" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C129" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C130" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C131" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C132" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C133" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>